<commit_message>
feat (phiên làm việc): hiệu chỉnh import excel + bắn thông báo từ nhập liệu đột xuất+ bổ sung
</commit_message>
<xml_diff>
--- a/ECP_V2.WebApplication/Content/MauNhapLieu/HPPC/Dvibc-Bsung.xlsx
+++ b/ECP_V2.WebApplication/Content/MauNhapLieu/HPPC/Dvibc-Bsung.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A7DD21-6912-48EA-988B-8D85B02B324C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9630"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bs- ngay (M-Dvi)" sheetId="61" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>Nội dung công việc</t>
   </si>
@@ -243,16 +244,28 @@
   </si>
   <si>
     <t>Công việc rửa sứ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hình thức kiểm tra hiện trường	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đại diện Đoàn KT hiện trường	</t>
+  </si>
+  <si>
+    <t>Kiểm tra đầu giờ</t>
+  </si>
+  <si>
+    <t>Bùi Duy Đức-PGĐ ĐL - 0963556777</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;&quot;?&quot;&quot;?&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -425,7 +438,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -435,6 +448,15 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Times New Roman"/>
     </font>
   </fonts>
@@ -587,50 +609,50 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,112 +688,125 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="49" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="Comma 2" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 11" xfId="3"/>
-    <cellStyle name="Normal 2 12" xfId="4"/>
-    <cellStyle name="Normal 2 13" xfId="5"/>
-    <cellStyle name="Normal 2 14" xfId="6"/>
-    <cellStyle name="Normal 2 15" xfId="7"/>
-    <cellStyle name="Normal 2 16" xfId="8"/>
-    <cellStyle name="Normal 2 17" xfId="9"/>
-    <cellStyle name="Normal 2 18" xfId="10"/>
-    <cellStyle name="Normal 2 19" xfId="11"/>
-    <cellStyle name="Normal 2 2" xfId="12"/>
-    <cellStyle name="Normal 2 20" xfId="13"/>
-    <cellStyle name="Normal 2 21" xfId="14"/>
-    <cellStyle name="Normal 2 22" xfId="15"/>
-    <cellStyle name="Normal 2 23" xfId="16"/>
-    <cellStyle name="Normal 2 24" xfId="17"/>
-    <cellStyle name="Normal 2 25" xfId="18"/>
-    <cellStyle name="Normal 2 26" xfId="19"/>
-    <cellStyle name="Normal 2 27" xfId="20"/>
-    <cellStyle name="Normal 2 28" xfId="21"/>
-    <cellStyle name="Normal 2 29" xfId="22"/>
-    <cellStyle name="Normal 2 3" xfId="23"/>
-    <cellStyle name="Normal 2 30" xfId="24"/>
-    <cellStyle name="Normal 2 31" xfId="25"/>
-    <cellStyle name="Normal 2 32" xfId="26"/>
-    <cellStyle name="Normal 2 33" xfId="27"/>
-    <cellStyle name="Normal 2 34" xfId="28"/>
-    <cellStyle name="Normal 2 37" xfId="29"/>
-    <cellStyle name="Normal 2 38" xfId="30"/>
-    <cellStyle name="Normal 2 39" xfId="31"/>
-    <cellStyle name="Normal 2 40" xfId="32"/>
-    <cellStyle name="Normal 2 41" xfId="33"/>
-    <cellStyle name="Normal 2 42" xfId="34"/>
-    <cellStyle name="Normal 2 43" xfId="35"/>
-    <cellStyle name="Normal 2 44" xfId="36"/>
-    <cellStyle name="Normal 2 46" xfId="37"/>
-    <cellStyle name="Normal 2 47" xfId="38"/>
-    <cellStyle name="Normal 2 48" xfId="39"/>
-    <cellStyle name="Normal 2 49" xfId="40"/>
-    <cellStyle name="Normal 2 50" xfId="41"/>
-    <cellStyle name="Normal 2 51" xfId="42"/>
-    <cellStyle name="Normal 2 52" xfId="43"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="47"/>
-    <cellStyle name="Normal 7" xfId="48"/>
-    <cellStyle name="Normal_Sheet1" xfId="49"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 12" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 13" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 14" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 15" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 16" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 17" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 18" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 2 19" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 20" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2 21" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2 22" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 23" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 24" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2 25" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 26" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 27" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 2 28" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 2 29" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 2 30" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 2 31" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 2 32" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 2 33" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 2 34" xfId="28" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal 2 37" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Normal 2 38" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Normal 2 39" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Normal 2 40" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Normal 2 41" xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Normal 2 42" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Normal 2 43" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Normal 2 44" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 2 46" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 2 47" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 48" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 2 49" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 2 50" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 2 51" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 2 52" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Normal 6" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 7" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -803,7 +838,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Connector 4"/>
+        <xdr:cNvPr id="2" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -847,7 +888,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40140" name="Line 1"/>
+        <xdr:cNvPr id="40140" name="Line 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000CC9C0000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeShapeType="1"/>
         </xdr:cNvSpPr>
@@ -884,7 +931,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Bc-Tuần (M-Dvi)"/>
@@ -928,9 +975,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -968,9 +1015,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1005,7 +1052,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1040,7 +1087,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1213,14 +1260,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,56 +1294,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="4"/>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
       <c r="S1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="4"/>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
       <c r="S2" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="47" t="s">
+      <c r="T2" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="4"/>
       <c r="F3" s="11"/>
       <c r="G3" s="4"/>
@@ -1316,12 +1363,12 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
       <c r="E4" s="4"/>
       <c r="F4" s="11"/>
       <c r="G4" s="4"/>
@@ -1335,10 +1382,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="12"/>
       <c r="F5" s="11"/>
       <c r="G5" s="4"/>
@@ -1358,58 +1405,58 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
       <c r="S6" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
       <c r="S7" s="28" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
       <c r="S8" s="28" t="s">
         <v>32</v>
       </c>
@@ -1467,6 +1514,12 @@
       <c r="R9" s="27" t="s">
         <v>67</v>
       </c>
+      <c r="S9" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="T9" s="52" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
@@ -1523,28 +1576,36 @@
       <c r="R10" s="20">
         <v>18</v>
       </c>
+      <c r="S10" s="48">
+        <v>19</v>
+      </c>
+      <c r="T10" s="48">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:20" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
       <c r="P11" s="23"/>
       <c r="Q11" s="23"/>
       <c r="R11" s="23"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
     </row>
     <row r="12" spans="1:20" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
@@ -1591,11 +1652,17 @@
         <v>52</v>
       </c>
       <c r="P12" s="23"/>
-      <c r="Q12" s="46" t="s">
+      <c r="Q12" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="R12" s="46" t="s">
+      <c r="R12" s="30" t="s">
         <v>69</v>
+      </c>
+      <c r="S12" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="T12" s="50" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1645,11 +1712,17 @@
       <c r="P13" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="Q13" s="46" t="s">
+      <c r="Q13" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="R13" s="46" t="s">
+      <c r="R13" s="30" t="s">
         <v>69</v>
+      </c>
+      <c r="S13" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="T13" s="50" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1695,11 +1768,17 @@
         <v>31</v>
       </c>
       <c r="P14" s="23"/>
-      <c r="Q14" s="46" t="s">
+      <c r="Q14" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="R14" s="46" t="s">
+      <c r="R14" s="30" t="s">
         <v>69</v>
+      </c>
+      <c r="S14" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="T14" s="50" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1721,6 +1800,8 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
       <c r="R15" s="23"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
     </row>
     <row r="16" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
@@ -1741,51 +1822,53 @@
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
       <c r="R16" s="23"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="51"/>
     </row>
     <row r="17" spans="1:11" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="14"/>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="36" t="s">
+      <c r="F17" s="36"/>
+      <c r="G17" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="36"/>
+      <c r="H17" s="33"/>
       <c r="I17" s="22"/>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="44"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" s="7" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="14"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="34" t="s">
+      <c r="J18" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="K18" s="34"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="14"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
@@ -1796,11 +1879,11 @@
       <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="14"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -1811,11 +1894,11 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="14"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
@@ -1826,11 +1909,11 @@
       <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="14"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
@@ -1842,6 +1925,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="A8:L8"/>
@@ -1855,14 +1946,6 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.11811023622047245" right="0" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1871,7 +1954,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>